<commit_message>
Update data of interest to use codes for mh_prior and belong2
</commit_message>
<xml_diff>
--- a/Data_of_interest_2023_05_22.xlsx
+++ b/Data_of_interest_2023_05_22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c35a92d2fb410ac3/Documents/GitHub/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyrie\github\queer-edu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{85F9E1CA-059B-4999-AE57-21C7F796D61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F7696F-2A63-4160-B7FF-F62550414526}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A56A08-476A-447C-99B4-EE7797302ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28755" yWindow="2340" windowWidth="13905" windowHeight="15510" xr2:uid="{43E0F8E0-77BC-4B97-8821-C44A17F69E85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43E0F8E0-77BC-4B97-8821-C44A17F69E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="211">
   <si>
     <t>Section</t>
   </si>
@@ -434,9 +434,6 @@
     <t>5=Disagree</t>
   </si>
   <si>
-    <t>At my school, I feel that students’ mental and emotional well-being is a priority.</t>
-  </si>
-  <si>
     <t>At my school, the administration is listening to the concerns of students when it comes to health and wellness.</t>
   </si>
   <si>
@@ -605,9 +602,6 @@
     <t>persist</t>
   </si>
   <si>
-    <t>Q12_3_1</t>
-  </si>
-  <si>
     <t>aca_impa</t>
   </si>
   <si>
@@ -669,6 +663,12 @@
   </si>
   <si>
     <t>fincur</t>
+  </si>
+  <si>
+    <t>mh_prior</t>
+  </si>
+  <si>
+    <t>belong2</t>
   </si>
 </sst>
 </file>
@@ -717,19 +717,19 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1047,20 +1047,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367990F3-F67E-4012-8396-553FF586656C}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.76953125" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.76953125" style="2"/>
-    <col min="2" max="2" width="36.81640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="19.76953125" style="2"/>
+    <col min="1" max="1" width="19.7109375" style="2"/>
+    <col min="2" max="2" width="36.85546875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="19.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,21 +1068,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.65">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1090,10 +1090,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="28.5" x14ac:dyDescent="0.65">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -1113,7 +1113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="42.75" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:26" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>11</v>
@@ -1148,7 +1148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -1189,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>32</v>
@@ -1221,7 +1221,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
@@ -1247,7 +1247,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="42.75" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:26" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>48</v>
@@ -1279,10 +1279,10 @@
         <v>54</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="28.5" x14ac:dyDescent="0.65">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>47</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>56</v>
@@ -1314,7 +1314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="57" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:26" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>64</v>
@@ -1346,7 +1346,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="71.25" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:26" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>72</v>
@@ -1375,7 +1375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="71.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>78</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>72</v>
@@ -1404,7 +1404,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="57" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>81</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>83</v>
@@ -1427,7 +1427,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="57.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:26" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>81</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>88</v>
@@ -1450,12 +1450,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="57.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:26" ht="57.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>93</v>
@@ -1527,12 +1527,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="71.25" x14ac:dyDescent="0.65">
+    <row r="17" spans="2:17" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>117</v>
@@ -1562,11 +1562,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="42.75" x14ac:dyDescent="0.65">
+    <row r="18" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="D18" s="4" t="s">
         <v>127</v>
       </c>
@@ -1586,12 +1588,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="43.25" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:17" ht="57.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>127</v>
@@ -1612,12 +1614,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="57.5" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:17" ht="57.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>127</v>
@@ -1638,111 +1640,111 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="57.5" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:17" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="43.25" x14ac:dyDescent="0.75">
-      <c r="B22" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" ht="85.5" x14ac:dyDescent="0.65">
-      <c r="B23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" ht="29" x14ac:dyDescent="0.75">
+    <row r="24" spans="2:17" ht="72" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>127</v>
@@ -1759,16 +1761,13 @@
       <c r="H24" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" ht="71.75" x14ac:dyDescent="0.75">
+    </row>
+    <row r="25" spans="2:17" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>127</v>
@@ -1785,159 +1784,136 @@
       <c r="H25" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="26" spans="2:17" ht="43.25" x14ac:dyDescent="0.75">
+      <c r="I25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" ht="42.75" x14ac:dyDescent="0.65">
-      <c r="B27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" ht="85.5" x14ac:dyDescent="0.65">
-      <c r="B28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" ht="85.5" x14ac:dyDescent="0.65">
+    </row>
+    <row r="29" spans="2:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" ht="85.5" x14ac:dyDescent="0.65">
-      <c r="B30" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>